<commit_message>
feat: Make final scraper
</commit_message>
<xml_diff>
--- a/Tiempos.xlsx
+++ b/Tiempos.xlsx
@@ -1,28 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26102"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfval\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BCRP\Codigos\GraphQL-Facebook-Marketplace-Ropa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="889" documentId="8_{46005872-38E0-40D7-9895-8AB5FAF4F425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1C06227-768C-46FF-BFFE-7271D29BC678}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB76CFE-D791-41CF-A565-B750330EA9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{30FB3611-AEDD-4647-A50F-D554F445B149}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electrodomesticos" sheetId="1" r:id="rId1"/>
-    <sheet name="Vestimenta" sheetId="3" r:id="rId2"/>
-    <sheet name="Vehiculos" sheetId="2" r:id="rId3"/>
+    <sheet name="Vestimenta" sheetId="2" r:id="rId2"/>
+    <sheet name="Vehiculos" sheetId="3" r:id="rId3"/>
     <sheet name="Ropa" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -211,7 +208,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,7 +271,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -294,7 +291,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,14 +603,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEFAE3E9-BAD1-4C01-981E-02727E63BE50}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="4" width="14.28515625" customWidth="1"/>
@@ -626,7 +623,7 @@
     <col min="11" max="11" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,12 +658,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2">
-        <v>0.37787037037037036</v>
+        <v>0.37787037037037041</v>
       </c>
       <c r="C2" s="2">
         <v>0.39280092592592591</v>
@@ -678,22 +675,22 @@
         <v>21.495999999999999</v>
       </c>
       <c r="F2">
-        <f>D2/E2</f>
+        <f t="shared" ref="F2:F39" si="0">D2/E2</f>
         <v>8.9318943059173801</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2">
-        <v>0.42150462962962965</v>
+        <v>0.42150462962962959</v>
       </c>
       <c r="C3" s="2">
-        <v>0.44690972222222225</v>
+        <v>0.44690972222222219</v>
       </c>
       <c r="D3">
         <v>285</v>
@@ -702,14 +699,14 @@
         <v>32.274999999999999</v>
       </c>
       <c r="F3">
-        <f>D3/E3</f>
+        <f t="shared" si="0"/>
         <v>8.8303640588690939</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -717,7 +714,7 @@
         <v>0.69374999999999998</v>
       </c>
       <c r="C4" s="2">
-        <v>0.71810185185185194</v>
+        <v>0.71810185185185182</v>
       </c>
       <c r="D4">
         <v>310</v>
@@ -726,22 +723,22 @@
         <v>35.064999999999998</v>
       </c>
       <c r="F4">
-        <f>D4/E4</f>
+        <f t="shared" si="0"/>
         <v>8.8407243690289476</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2">
-        <v>0.7672337962962964</v>
+        <v>0.76723379629629629</v>
       </c>
       <c r="C5" s="2">
-        <v>0.79636574074074085</v>
+        <v>0.79636574074074074</v>
       </c>
       <c r="D5">
         <v>370</v>
@@ -750,14 +747,14 @@
         <v>41.945</v>
       </c>
       <c r="F5">
-        <f>D5/E5</f>
+        <f t="shared" si="0"/>
         <v>8.8210752175467881</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -774,19 +771,19 @@
         <v>2.7989999999999999</v>
       </c>
       <c r="F6">
-        <f>D6/E6</f>
+        <f t="shared" si="0"/>
         <v>7.1454090746695247</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>0.55503472222222217</v>
+        <v>0.55503472222222228</v>
       </c>
       <c r="C7" s="2">
         <v>0.55688657407407405</v>
@@ -798,14 +795,14 @@
         <v>2.6669999999999998</v>
       </c>
       <c r="F7">
-        <f>D7/E7</f>
+        <f t="shared" si="0"/>
         <v>7.4990626171728536</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -822,14 +819,14 @@
         <v>2.6619999999999999</v>
       </c>
       <c r="F8">
-        <f>D8/E8</f>
+        <f t="shared" si="0"/>
         <v>7.5131480090157776</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -837,7 +834,7 @@
         <v>0.68917824074074074</v>
       </c>
       <c r="C9" s="2">
-        <v>0.70613425925925932</v>
+        <v>0.70613425925925921</v>
       </c>
       <c r="D9">
         <v>215</v>
@@ -846,7 +843,7 @@
         <v>24.402999999999999</v>
       </c>
       <c r="F9">
-        <f>D9/E9</f>
+        <f t="shared" si="0"/>
         <v>8.8103921648977597</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -856,7 +853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -864,7 +861,7 @@
         <v>0.75542824074074078</v>
       </c>
       <c r="C10" s="2">
-        <v>0.76962962962962955</v>
+        <v>0.76962962962962966</v>
       </c>
       <c r="D10">
         <v>44</v>
@@ -873,7 +870,7 @@
         <v>4.9870000000000001</v>
       </c>
       <c r="F10">
-        <f>D10/E10</f>
+        <f t="shared" si="0"/>
         <v>8.8229396430719866</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -883,12 +880,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>0.71458333333333324</v>
+        <v>0.71458333333333335</v>
       </c>
       <c r="C11" s="2">
         <v>0.72192129629629631</v>
@@ -900,7 +897,7 @@
         <v>10.567</v>
       </c>
       <c r="F11">
-        <f>D11/E11</f>
+        <f t="shared" si="0"/>
         <v>5.5834200813854453</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -910,7 +907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -927,7 +924,7 @@
         <v>22.814</v>
       </c>
       <c r="F12">
-        <f>D12/E12</f>
+        <f t="shared" si="0"/>
         <v>8.8103795914789167</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -937,7 +934,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -954,7 +951,7 @@
         <v>13.574</v>
       </c>
       <c r="F13">
-        <f>D13/E13</f>
+        <f t="shared" si="0"/>
         <v>8.8404302342714018</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -964,12 +961,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>0.76962962962962955</v>
+        <v>0.76962962962962966</v>
       </c>
       <c r="C14" s="2">
         <v>0.78364583333333337</v>
@@ -981,7 +978,7 @@
         <v>11.551</v>
       </c>
       <c r="F14">
-        <f>D14/E14</f>
+        <f t="shared" si="0"/>
         <v>8.8304042940005196</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -991,12 +988,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <v>0.72168981481481476</v>
+        <v>0.72168981481481487</v>
       </c>
       <c r="C15" s="10">
         <v>0.74616898148148147</v>
@@ -1008,7 +1005,7 @@
         <v>31.257000000000001</v>
       </c>
       <c r="F15">
-        <f>D15/E15</f>
+        <f t="shared" si="0"/>
         <v>8.8300220750551865</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -1021,7 +1018,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1029,7 +1026,7 @@
         <v>0.84520833333333334</v>
       </c>
       <c r="C16" s="2">
-        <v>0.87418981481481473</v>
+        <v>0.87418981481481484</v>
       </c>
       <c r="D16">
         <v>43</v>
@@ -1038,7 +1035,7 @@
         <v>41.44</v>
       </c>
       <c r="F16" s="11">
-        <f>D16/E16</f>
+        <f t="shared" si="0"/>
         <v>1.0376447876447876</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -1051,7 +1048,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15">
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1059,7 +1056,7 @@
         <v>0.51045138888888886</v>
       </c>
       <c r="C17" s="2">
-        <v>0.52951388888888895</v>
+        <v>0.52951388888888884</v>
       </c>
       <c r="D17">
         <v>59</v>
@@ -1068,7 +1065,7 @@
         <v>27.45</v>
       </c>
       <c r="F17" s="11">
-        <f>D17/E17</f>
+        <f t="shared" si="0"/>
         <v>2.1493624772313296</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -1084,7 +1081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15">
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1092,7 +1089,7 @@
         <v>0.54578703703703701</v>
       </c>
       <c r="C18" s="2">
-        <v>0.55908564814814821</v>
+        <v>0.5590856481481481</v>
       </c>
       <c r="D18">
         <v>37</v>
@@ -1101,7 +1098,7 @@
         <v>19.146999999999998</v>
       </c>
       <c r="F18" s="11">
-        <f>D18/E18</f>
+        <f t="shared" si="0"/>
         <v>1.9324176111140128</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1114,12 +1111,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15">
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.88370370370370377</v>
+        <v>0.88370370370370366</v>
       </c>
       <c r="C19" s="2">
         <v>0.90248842592592593</v>
@@ -1131,7 +1128,7 @@
         <v>27.05</v>
       </c>
       <c r="F19" s="12">
-        <f>D19/E19</f>
+        <f t="shared" si="0"/>
         <v>5.0277264325323472</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -1147,7 +1144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1164,7 +1161,7 @@
         <v>23.408999999999999</v>
       </c>
       <c r="F20" s="12">
-        <f>D20/E20</f>
+        <f t="shared" si="0"/>
         <v>6.7495407749156309</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -1177,12 +1174,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15">
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="2">
-        <v>0.51673611111111117</v>
+        <v>0.51673611111111106</v>
       </c>
       <c r="C21" s="2">
         <v>0.53420138888888891</v>
@@ -1194,7 +1191,7 @@
         <v>25.152999999999999</v>
       </c>
       <c r="F21" s="12">
-        <f>D21/E21</f>
+        <f t="shared" si="0"/>
         <v>5.2081262672444639</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -1210,12 +1207,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15">
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="2">
-        <v>0.55328703703703697</v>
+        <v>0.55328703703703708</v>
       </c>
       <c r="C22" s="2">
         <v>0.56722222222222218</v>
@@ -1227,7 +1224,7 @@
         <v>20.061</v>
       </c>
       <c r="F22" s="12">
-        <f>D22/E22</f>
+        <f t="shared" si="0"/>
         <v>3.3896615323264045</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -1243,7 +1240,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15">
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1260,7 +1257,7 @@
         <v>6.6109999999999998</v>
       </c>
       <c r="F23" s="12">
-        <f>D23/E23</f>
+        <f t="shared" si="0"/>
         <v>5.8992588110724551</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -1279,7 +1276,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15">
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1296,7 +1293,7 @@
         <v>27.513000000000002</v>
       </c>
       <c r="F24" s="12">
-        <f>D24/E24</f>
+        <f t="shared" si="0"/>
         <v>6.615054701413877</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -1309,7 +1306,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15">
+    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1326,7 +1323,7 @@
         <v>45.267000000000003</v>
       </c>
       <c r="F25" s="12">
-        <f>D25/E25</f>
+        <f t="shared" si="0"/>
         <v>4.3298650230852491</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -1342,7 +1339,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15">
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1350,7 +1347,7 @@
         <v>0.89288194444444446</v>
       </c>
       <c r="C26" s="2">
-        <v>0.93597222222222232</v>
+        <v>0.93597222222222221</v>
       </c>
       <c r="D26">
         <v>264</v>
@@ -1359,7 +1356,7 @@
         <v>51.662999999999997</v>
       </c>
       <c r="F26" s="12">
-        <f>D26/E26</f>
+        <f t="shared" si="0"/>
         <v>5.1100400673596198</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -1375,7 +1372,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15">
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>19.859000000000002</v>
       </c>
       <c r="F27" s="12">
-        <f>D27/E27</f>
+        <f t="shared" si="0"/>
         <v>6.6972153683468445</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -1405,12 +1402,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15">
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="2">
-        <v>0.94422453703703713</v>
+        <v>0.94422453703703701</v>
       </c>
       <c r="C28" s="2">
         <v>0.96001157407407411</v>
@@ -1422,7 +1419,7 @@
         <v>22.727</v>
       </c>
       <c r="F28" s="12">
-        <f>D28/E28</f>
+        <f t="shared" si="0"/>
         <v>6.9080828969947641</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -1435,7 +1432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15">
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1449,7 @@
         <v>40.076999999999998</v>
       </c>
       <c r="F29" s="12">
-        <f>D29/E29</f>
+        <f t="shared" si="0"/>
         <v>6.1132320283454353</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -1465,7 +1462,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15">
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1470,7 @@
         <v>0.84065972222222218</v>
       </c>
       <c r="C30" s="2">
-        <v>0.86887731481481489</v>
+        <v>0.86887731481481478</v>
       </c>
       <c r="D30">
         <v>276</v>
@@ -1482,7 +1479,7 @@
         <v>40.630000000000003</v>
       </c>
       <c r="F30" s="12">
-        <f>D30/E30</f>
+        <f t="shared" si="0"/>
         <v>6.7930100910657147</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -1495,7 +1492,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15">
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1512,7 +1509,7 @@
         <v>33.119999999999997</v>
       </c>
       <c r="F31" s="12">
-        <f>D31/E31</f>
+        <f t="shared" si="0"/>
         <v>6.9142512077294693</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -1525,12 +1522,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15">
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="2">
-        <v>0.90309027777777784</v>
+        <v>0.90309027777777773</v>
       </c>
       <c r="C32" s="2">
         <v>0.93056712962962962</v>
@@ -1542,7 +1539,7 @@
         <v>39.576000000000001</v>
       </c>
       <c r="F32" s="12">
-        <f>D32/E32</f>
+        <f t="shared" si="0"/>
         <v>6.9233879118657775</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -1555,7 +1552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15">
+    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1563,7 +1560,7 @@
         <v>0.87599537037037034</v>
       </c>
       <c r="C33" s="2">
-        <v>0.90354166666666658</v>
+        <v>0.90354166666666669</v>
       </c>
       <c r="D33">
         <v>277</v>
@@ -1572,7 +1569,7 @@
         <v>39.664000000000001</v>
       </c>
       <c r="F33" s="12">
-        <f>D33/E33</f>
+        <f t="shared" si="0"/>
         <v>6.9836627672448568</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -1585,12 +1582,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15">
+    <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="2">
-        <v>0.92202546296296306</v>
+        <v>0.92202546296296295</v>
       </c>
       <c r="C34" s="2">
         <v>0.94923611111111106</v>
@@ -1602,7 +1599,7 @@
         <v>39.177999999999997</v>
       </c>
       <c r="F34" s="12">
-        <f>D34/E34</f>
+        <f t="shared" si="0"/>
         <v>6.9426719077033034</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -1615,7 +1612,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15">
+    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -1632,7 +1629,7 @@
         <v>35.725999999999999</v>
       </c>
       <c r="F35" s="12">
-        <f>D35/E35</f>
+        <f t="shared" si="0"/>
         <v>6.9697139338297038</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -1648,7 +1645,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15">
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -1665,7 +1662,7 @@
         <v>40.066000000000003</v>
       </c>
       <c r="F36" s="12">
-        <f>D36/E36</f>
+        <f t="shared" si="0"/>
         <v>6.9385513902061593</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -1678,7 +1675,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15">
+    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -1695,7 +1692,7 @@
         <v>19.959</v>
       </c>
       <c r="F37" s="12">
-        <f>D37/E37</f>
+        <f t="shared" si="0"/>
         <v>6.7137632145899095</v>
       </c>
       <c r="G37" s="3" t="s">
@@ -1708,7 +1705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15">
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -1725,7 +1722,7 @@
         <v>21.908999999999999</v>
       </c>
       <c r="F38" s="12">
-        <f>D38/E38</f>
+        <f t="shared" si="0"/>
         <v>6.8921447806837373</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -1738,7 +1735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15">
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1755,7 +1752,7 @@
         <v>73.334999999999994</v>
       </c>
       <c r="F39" s="12">
-        <f>D39/E39</f>
+        <f t="shared" si="0"/>
         <v>6.7225744869434791</v>
       </c>
       <c r="G39" s="3" t="s">
@@ -1768,7 +1765,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1797,526 +1794,526 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E41" s="9"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E46" s="9"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E47" s="9"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E48" s="9"/>
     </row>
-    <row r="49" spans="5:5">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="5:5">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E50" s="9"/>
     </row>
-    <row r="51" spans="5:5">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="5:5">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E52" s="9"/>
     </row>
-    <row r="53" spans="5:5">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="5:5">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="5:5">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="5:5">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="5:5">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="5:5">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E58" s="9"/>
     </row>
-    <row r="59" spans="5:5">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="5:5">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E60" s="9"/>
     </row>
-    <row r="61" spans="5:5">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="5:5">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E62" s="9"/>
     </row>
-    <row r="63" spans="5:5">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E63" s="9"/>
     </row>
-    <row r="64" spans="5:5">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E64" s="9"/>
     </row>
-    <row r="65" spans="5:5">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65" s="9"/>
     </row>
-    <row r="66" spans="5:5">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E66" s="9"/>
     </row>
-    <row r="67" spans="5:5">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E67" s="9"/>
     </row>
-    <row r="68" spans="5:5">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E68" s="9"/>
     </row>
-    <row r="69" spans="5:5">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E69" s="9"/>
     </row>
-    <row r="70" spans="5:5">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E70" s="9"/>
     </row>
-    <row r="71" spans="5:5">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="5:5">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E72" s="9"/>
     </row>
-    <row r="73" spans="5:5">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="5:5">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="5:5">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E75" s="9"/>
     </row>
-    <row r="76" spans="5:5">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E76" s="9"/>
     </row>
-    <row r="77" spans="5:5">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="5:5">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E78" s="9"/>
     </row>
-    <row r="79" spans="5:5">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E79" s="9"/>
     </row>
-    <row r="80" spans="5:5">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E80" s="9"/>
     </row>
-    <row r="81" spans="5:5">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" s="9"/>
     </row>
-    <row r="82" spans="5:5">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E82" s="9"/>
     </row>
-    <row r="83" spans="5:5">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="5:5">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E84" s="9"/>
     </row>
-    <row r="85" spans="5:5">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E85" s="9"/>
     </row>
-    <row r="86" spans="5:5">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E86" s="9"/>
     </row>
-    <row r="87" spans="5:5">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E87" s="9"/>
     </row>
-    <row r="88" spans="5:5">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E88" s="9"/>
     </row>
-    <row r="89" spans="5:5">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E89" s="9"/>
     </row>
-    <row r="90" spans="5:5">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E90" s="9"/>
     </row>
-    <row r="91" spans="5:5">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="5:5">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E92" s="9"/>
     </row>
-    <row r="93" spans="5:5">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="5:5">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E94" s="9"/>
     </row>
-    <row r="95" spans="5:5">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E95" s="9"/>
     </row>
-    <row r="96" spans="5:5">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E96" s="9"/>
     </row>
-    <row r="97" spans="5:5">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="9"/>
     </row>
-    <row r="98" spans="5:5">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="9"/>
     </row>
-    <row r="99" spans="5:5">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="9"/>
     </row>
-    <row r="100" spans="5:5">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="9"/>
     </row>
-    <row r="101" spans="5:5">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="9"/>
     </row>
-    <row r="102" spans="5:5">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="9"/>
     </row>
-    <row r="103" spans="5:5">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="9"/>
     </row>
-    <row r="104" spans="5:5">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="9"/>
     </row>
-    <row r="105" spans="5:5">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="9"/>
     </row>
-    <row r="106" spans="5:5">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="9"/>
     </row>
-    <row r="107" spans="5:5">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="9"/>
     </row>
-    <row r="108" spans="5:5">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="9"/>
     </row>
-    <row r="109" spans="5:5">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="9"/>
     </row>
-    <row r="110" spans="5:5">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="9"/>
     </row>
-    <row r="111" spans="5:5">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="9"/>
     </row>
-    <row r="112" spans="5:5">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="9"/>
     </row>
-    <row r="113" spans="5:5">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="9"/>
     </row>
-    <row r="114" spans="5:5">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="9"/>
     </row>
-    <row r="115" spans="5:5">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="9"/>
     </row>
-    <row r="116" spans="5:5">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="9"/>
     </row>
-    <row r="117" spans="5:5">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="9"/>
     </row>
-    <row r="118" spans="5:5">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="9"/>
     </row>
-    <row r="119" spans="5:5">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="9"/>
     </row>
-    <row r="120" spans="5:5">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="9"/>
     </row>
-    <row r="121" spans="5:5">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="9"/>
     </row>
-    <row r="122" spans="5:5">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="9"/>
     </row>
-    <row r="123" spans="5:5">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="9"/>
     </row>
-    <row r="124" spans="5:5">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="9"/>
     </row>
-    <row r="125" spans="5:5">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" s="9"/>
     </row>
-    <row r="126" spans="5:5">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E126" s="9"/>
     </row>
-    <row r="127" spans="5:5">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E127" s="9"/>
     </row>
-    <row r="128" spans="5:5">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E128" s="9"/>
     </row>
-    <row r="129" spans="5:5">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" s="9"/>
     </row>
-    <row r="130" spans="5:5">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" s="9"/>
     </row>
-    <row r="131" spans="5:5">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" s="9"/>
     </row>
-    <row r="132" spans="5:5">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E132" s="9"/>
     </row>
-    <row r="133" spans="5:5">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E133" s="9"/>
     </row>
-    <row r="134" spans="5:5">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E134" s="9"/>
     </row>
-    <row r="135" spans="5:5">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E135" s="9"/>
     </row>
-    <row r="136" spans="5:5">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E136" s="9"/>
     </row>
-    <row r="137" spans="5:5">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E137" s="9"/>
     </row>
-    <row r="138" spans="5:5">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E138" s="9"/>
     </row>
-    <row r="139" spans="5:5">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E139" s="9"/>
     </row>
-    <row r="140" spans="5:5">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E140" s="9"/>
     </row>
-    <row r="141" spans="5:5">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E141" s="9"/>
     </row>
-    <row r="142" spans="5:5">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E142" s="9"/>
     </row>
-    <row r="143" spans="5:5">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E143" s="9"/>
     </row>
-    <row r="144" spans="5:5">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E144" s="9"/>
     </row>
-    <row r="145" spans="5:5">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" s="9"/>
     </row>
-    <row r="146" spans="5:5">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" s="9"/>
     </row>
-    <row r="147" spans="5:5">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" s="9"/>
     </row>
-    <row r="148" spans="5:5">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" s="9"/>
     </row>
-    <row r="149" spans="5:5">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" s="9"/>
     </row>
-    <row r="150" spans="5:5">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" s="9"/>
     </row>
-    <row r="151" spans="5:5">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E151" s="9"/>
     </row>
-    <row r="152" spans="5:5">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E152" s="9"/>
     </row>
-    <row r="153" spans="5:5">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E153" s="9"/>
     </row>
-    <row r="154" spans="5:5">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E154" s="9"/>
     </row>
-    <row r="155" spans="5:5">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E155" s="9"/>
     </row>
-    <row r="156" spans="5:5">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E156" s="9"/>
     </row>
-    <row r="157" spans="5:5">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E157" s="9"/>
     </row>
-    <row r="158" spans="5:5">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E158" s="9"/>
     </row>
-    <row r="159" spans="5:5">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E159" s="9"/>
     </row>
-    <row r="160" spans="5:5">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E160" s="9"/>
     </row>
-    <row r="161" spans="5:5">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E161" s="9"/>
     </row>
-    <row r="162" spans="5:5">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E162" s="9"/>
     </row>
-    <row r="163" spans="5:5">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E163" s="9"/>
     </row>
-    <row r="164" spans="5:5">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E164" s="9"/>
     </row>
-    <row r="165" spans="5:5">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E165" s="9"/>
     </row>
-    <row r="166" spans="5:5">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E166" s="9"/>
     </row>
-    <row r="167" spans="5:5">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E167" s="9"/>
     </row>
-    <row r="168" spans="5:5">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E168" s="9"/>
     </row>
-    <row r="169" spans="5:5">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E169" s="9"/>
     </row>
-    <row r="170" spans="5:5">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E170" s="9"/>
     </row>
-    <row r="171" spans="5:5">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E171" s="9"/>
     </row>
-    <row r="172" spans="5:5">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E172" s="9"/>
     </row>
-    <row r="173" spans="5:5">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E173" s="9"/>
     </row>
-    <row r="174" spans="5:5">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E174" s="9"/>
     </row>
-    <row r="175" spans="5:5">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E175" s="9"/>
     </row>
-    <row r="176" spans="5:5">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E176" s="9"/>
     </row>
-    <row r="177" spans="5:5">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E177" s="9"/>
     </row>
-    <row r="178" spans="5:5">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E178" s="9"/>
     </row>
-    <row r="179" spans="5:5">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E179" s="9"/>
     </row>
-    <row r="180" spans="5:5">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E180" s="9"/>
     </row>
-    <row r="181" spans="5:5">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E181" s="9"/>
     </row>
-    <row r="182" spans="5:5">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E182" s="9"/>
     </row>
-    <row r="183" spans="5:5">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E183" s="9"/>
     </row>
-    <row r="184" spans="5:5">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E184" s="9"/>
     </row>
-    <row r="185" spans="5:5">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E185" s="9"/>
     </row>
-    <row r="186" spans="5:5">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E186" s="9"/>
     </row>
-    <row r="187" spans="5:5">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E187" s="9"/>
     </row>
-    <row r="188" spans="5:5">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E188" s="9"/>
     </row>
-    <row r="189" spans="5:5">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E189" s="9"/>
     </row>
-    <row r="190" spans="5:5">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E190" s="9"/>
     </row>
-    <row r="191" spans="5:5">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E191" s="9"/>
     </row>
-    <row r="192" spans="5:5">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E192" s="9"/>
     </row>
-    <row r="193" spans="5:5">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E193" s="9"/>
     </row>
-    <row r="194" spans="5:5">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E194" s="9"/>
     </row>
-    <row r="195" spans="5:5">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E195" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{AE50987C-1DE7-4107-9F41-BEBC1835543A}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{B8478255-100F-4414-A09F-7EFA2D1AB8E7}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{FB51F7C9-14DB-4ED6-9035-73C1416B28C9}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{8DC0AC69-2F2E-4B00-9D4C-99185E4D718B}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{BE028F9C-AC45-4779-A69E-06A5D556463D}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{564597C5-8E2D-4C7C-AD9B-3CE4ABADAA74}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{2630BE51-AFF2-43D4-85A9-5084E83A0A8E}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{742A4E22-712F-4011-9757-5F1BA31C5780}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{37B1FA86-2D69-4266-B132-751DEE36F91F}"/>
-    <hyperlink ref="G11" r:id="rId10" xr:uid="{398EFAAD-1543-49B1-8D31-AE906F6AD5FD}"/>
-    <hyperlink ref="G12" r:id="rId11" xr:uid="{3361E90A-374E-426B-A5B7-DC64CB27471F}"/>
-    <hyperlink ref="G13" r:id="rId12" xr:uid="{781F36D4-7283-403F-A8A6-28A008440204}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{F688923D-F515-4463-BD51-D9A71160B407}"/>
-    <hyperlink ref="G15" r:id="rId14" xr:uid="{79292869-9E6D-418F-B21E-057F209C0E0C}"/>
-    <hyperlink ref="G16" r:id="rId15" xr:uid="{D9846B5D-384F-4959-86C2-35E116569A60}"/>
-    <hyperlink ref="G17" r:id="rId16" xr:uid="{2DED17A4-71DE-4AF4-AA55-F591C35F7347}"/>
-    <hyperlink ref="G18" r:id="rId17" xr:uid="{4E5E6E9B-B270-42CC-9473-6D8DB4DB2B5D}"/>
-    <hyperlink ref="G19" r:id="rId18" xr:uid="{499C070A-E876-490A-BAD7-B926C406A5F8}"/>
-    <hyperlink ref="G20" r:id="rId19" xr:uid="{6F7D0E87-FE30-4BEB-8203-44EBF8E8AD7A}"/>
-    <hyperlink ref="G21" r:id="rId20" xr:uid="{1FF1051C-A87C-46FC-AF4C-4F8E26362294}"/>
-    <hyperlink ref="G22" r:id="rId21" xr:uid="{5517F245-F897-4BB5-9B9B-67C090BD4607}"/>
-    <hyperlink ref="G23" r:id="rId22" xr:uid="{2BF38270-64BD-43A6-AFF7-C897B17F15F6}"/>
-    <hyperlink ref="G24" r:id="rId23" xr:uid="{4C278271-8849-46A8-B1C3-E9522B77BA6E}"/>
-    <hyperlink ref="G25" r:id="rId24" xr:uid="{BA7251A4-3386-450D-B53F-C0E78F92953D}"/>
-    <hyperlink ref="G26" r:id="rId25" xr:uid="{75380E7C-3AAE-4169-A109-E093B2290985}"/>
-    <hyperlink ref="G27" r:id="rId26" xr:uid="{3284D6B5-0055-4732-80CB-3E76FD52A97B}"/>
-    <hyperlink ref="G28" r:id="rId27" xr:uid="{D8F91106-8186-40DE-BF4C-C26C65E4D335}"/>
-    <hyperlink ref="G29" r:id="rId28" xr:uid="{D3FFFC3D-0AEF-4C7E-9DE2-20FC0CD28D03}"/>
-    <hyperlink ref="G30" r:id="rId29" xr:uid="{E98F58B3-2171-47C0-9CE3-D8F452153FE0}"/>
-    <hyperlink ref="G31" r:id="rId30" xr:uid="{02C48720-2619-4372-A5D6-A2D795E2B7FB}"/>
-    <hyperlink ref="G32" r:id="rId31" xr:uid="{E785E034-AF93-49D2-9983-D1B5F1A1D16A}"/>
-    <hyperlink ref="G33" r:id="rId32" xr:uid="{39BC3491-A800-4E96-9C7C-08C616D16751}"/>
-    <hyperlink ref="G34" r:id="rId33" xr:uid="{86924B9E-63DB-4EDC-BF2E-1212C7BC14C0}"/>
-    <hyperlink ref="G35" r:id="rId34" xr:uid="{64E7219E-FB16-41A8-8F39-E9A0E767A9FD}"/>
-    <hyperlink ref="G36" r:id="rId35" xr:uid="{0EED64AE-4019-4F53-B0CF-1435FC9CD86E}"/>
-    <hyperlink ref="G37" r:id="rId36" xr:uid="{0D1400D2-F8F3-487E-A507-A47101A4F748}"/>
-    <hyperlink ref="G38" r:id="rId37" xr:uid="{BBAE65BC-7127-4261-BDCC-93C53E4F94C9}"/>
-    <hyperlink ref="G39" r:id="rId38" xr:uid="{5DCD87AD-FC1C-4F86-AAF5-899BCAE33BCC}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="G36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="G37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="G38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="G39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId39"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB400271-0187-4A99-8B7F-136F5EE4567C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
@@ -2328,7 +2325,7 @@
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2363,7 +2360,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2380,14 +2377,14 @@
         <v>2.7130000000000001</v>
       </c>
       <c r="F2">
-        <f>D2/E2</f>
+        <f t="shared" ref="F2:F19" si="0">D2/E2</f>
         <v>7.3719130114264653</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2404,7 +2401,7 @@
         <v>7.6529999999999996</v>
       </c>
       <c r="F3">
-        <f>D3/E3</f>
+        <f t="shared" si="0"/>
         <v>7.8400627205017646</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -2414,15 +2411,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="2">
-        <v>0.92017361111111118</v>
+        <v>0.92017361111111107</v>
       </c>
       <c r="C4" s="2">
-        <v>0.93540509259259252</v>
+        <v>0.93540509259259264</v>
       </c>
       <c r="D4">
         <v>144</v>
@@ -2431,7 +2428,7 @@
         <v>21.92</v>
       </c>
       <c r="F4">
-        <f>D4/E4</f>
+        <f t="shared" si="0"/>
         <v>6.5693430656934302</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -2441,7 +2438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2458,7 +2455,7 @@
         <v>7.2629999999999999</v>
       </c>
       <c r="F5">
-        <f>D5/E5</f>
+        <f t="shared" si="0"/>
         <v>5.3696819496076005</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -2471,7 +2468,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2479,7 +2476,7 @@
         <v>0.87969907407407411</v>
       </c>
       <c r="C6" s="2">
-        <v>0.90771990740740749</v>
+        <v>0.90771990740740738</v>
       </c>
       <c r="D6">
         <v>271</v>
@@ -2488,7 +2485,7 @@
         <v>40.348999999999997</v>
       </c>
       <c r="F6">
-        <f>D6/E6</f>
+        <f t="shared" si="0"/>
         <v>6.7163994151032247</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -2501,7 +2498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2509,7 +2506,7 @@
         <v>0.57590277777777776</v>
       </c>
       <c r="C7" s="2">
-        <v>0.61534722222222216</v>
+        <v>0.61534722222222227</v>
       </c>
       <c r="D7">
         <v>539</v>
@@ -2518,7 +2515,7 @@
         <v>56.808</v>
       </c>
       <c r="F7">
-        <f>D7/E7</f>
+        <f t="shared" si="0"/>
         <v>9.4881002675679476</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -2534,7 +2531,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2542,7 +2539,7 @@
         <v>0.78917824074074072</v>
       </c>
       <c r="C8" s="2">
-        <v>0.82603009259259252</v>
+        <v>0.82603009259259264</v>
       </c>
       <c r="D8">
         <v>207</v>
@@ -2551,7 +2548,7 @@
         <v>53.067</v>
       </c>
       <c r="F8">
-        <f>D8/E8</f>
+        <f t="shared" si="0"/>
         <v>3.9007292667759623</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -2567,7 +2564,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2584,7 +2581,7 @@
         <v>19.884</v>
       </c>
       <c r="F9">
-        <f>D9/E9</f>
+        <f t="shared" si="0"/>
         <v>4.9788774894387444</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -2597,7 +2594,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2614,7 +2611,7 @@
         <v>14.675000000000001</v>
       </c>
       <c r="F10">
-        <f>D10/E10</f>
+        <f t="shared" si="0"/>
         <v>6.746166950596252</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -2630,12 +2627,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2">
-        <v>0.46260416666666665</v>
+        <v>0.46260416666666659</v>
       </c>
       <c r="C11" s="2">
         <v>0.47340277777777778</v>
@@ -2647,7 +2644,7 @@
         <v>15.555</v>
       </c>
       <c r="F11">
-        <f>D11/E11</f>
+        <f t="shared" si="0"/>
         <v>6.557377049180328</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -2660,15 +2657,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>0.99685185185185177</v>
+        <v>0.99685185185185188</v>
       </c>
       <c r="C12" s="2">
-        <v>1.1412037037037038E-2</v>
+        <v>1.141203703703704E-2</v>
       </c>
       <c r="D12">
         <v>137</v>
@@ -2677,7 +2674,7 @@
         <v>20.97</v>
       </c>
       <c r="F12">
-        <f>D12/E12</f>
+        <f t="shared" si="0"/>
         <v>6.5331425846447306</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -2690,7 +2687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2707,7 +2704,7 @@
         <v>14.704000000000001</v>
       </c>
       <c r="F13">
-        <f>D13/E13</f>
+        <f t="shared" si="0"/>
         <v>6.8008705114254617</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -2720,7 +2717,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2737,7 +2734,7 @@
         <v>42.975000000000001</v>
       </c>
       <c r="F14">
-        <f>D14/E14</f>
+        <f t="shared" si="0"/>
         <v>6.5386852821407793</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -2750,7 +2747,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2767,7 +2764,7 @@
         <v>34.661000000000001</v>
       </c>
       <c r="F15">
-        <f>D15/E15</f>
+        <f t="shared" si="0"/>
         <v>6.924208764894261</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -2780,7 +2777,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2797,7 +2794,7 @@
         <v>33.981000000000002</v>
       </c>
       <c r="F16">
-        <f>D16/E16</f>
+        <f t="shared" si="0"/>
         <v>7.0039139519143045</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -2810,12 +2807,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <v>0.80491898148148155</v>
+        <v>0.80491898148148144</v>
       </c>
       <c r="C17" s="2">
         <v>0.83187500000000003</v>
@@ -2827,7 +2824,7 @@
         <v>38.804000000000002</v>
       </c>
       <c r="F17">
-        <f>D17/E17</f>
+        <f t="shared" si="0"/>
         <v>6.9322750231934851</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -2843,7 +2840,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2860,7 +2857,7 @@
         <v>14.962</v>
       </c>
       <c r="F18">
-        <f>D18/E18</f>
+        <f t="shared" si="0"/>
         <v>6.6835984494051601</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -2873,7 +2870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2890,7 +2887,7 @@
         <v>83.872</v>
       </c>
       <c r="F19">
-        <f>D19/E19</f>
+        <f t="shared" si="0"/>
         <v>6.9152995040061045</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -2905,38 +2902,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{0A3AA25C-17FC-4CBB-A6BA-7D4BB0A95B69}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{F7AB846E-7AA8-4FFF-BFEA-801DC497205E}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{07786126-6E2A-43E5-BEEF-F3B59E8DA009}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{DA071F04-21C8-45EA-B893-8EFF53913875}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{8D7E1BBF-689D-4A28-9941-328EF85D1D27}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{6249CC7A-AF9E-4A42-8019-ACFF1A4A5912}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{293DD93B-F9EA-4879-8C3E-53C41CE06E88}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{788E98C8-BDC6-4902-99EC-664C6EB5EE24}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{513334E1-1A37-4189-BBB5-C40352520598}"/>
-    <hyperlink ref="G11" r:id="rId10" xr:uid="{A7C22F52-70FF-47ED-8289-029033789616}"/>
-    <hyperlink ref="G12" r:id="rId11" xr:uid="{355285D6-05EB-4576-9DEB-57421BD0670C}"/>
-    <hyperlink ref="G13" r:id="rId12" xr:uid="{2A5A86A1-0C56-45DF-89D2-650019B8A20C}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{D6A558D6-7B0C-49E0-915E-2BE31846F50A}"/>
-    <hyperlink ref="G15" r:id="rId14" xr:uid="{B1F31E52-C317-483F-932D-B51FA399377E}"/>
-    <hyperlink ref="G16" r:id="rId15" xr:uid="{6AD1B1C8-A26D-4533-ACBC-8830CBE63624}"/>
-    <hyperlink ref="G17" r:id="rId16" xr:uid="{D2500614-76E6-4269-A373-69507DCC9670}"/>
-    <hyperlink ref="G18" r:id="rId17" xr:uid="{78D29CFE-4C7C-448A-994F-71691B9B91C6}"/>
-    <hyperlink ref="G19" r:id="rId18" xr:uid="{357075F8-8F14-4D98-9445-B0CC98BC16C8}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="G14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="G15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="G16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="G17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="G18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="G19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E703AE-4E2F-4A2D-ACA2-43B028AFE9BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="4" width="14.28515625" customWidth="1"/>
@@ -2946,7 +2943,7 @@
     <col min="8" max="8" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -2972,22 +2969,22 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>44900</v>
       </c>
       <c r="B2" s="2">
-        <v>0.45208333333333334</v>
+        <v>0.45208333333333328</v>
       </c>
       <c r="C2" s="2">
-        <v>0.47291666666666665</v>
+        <v>0.47291666666666671</v>
       </c>
       <c r="D2">
         <v>202</v>
       </c>
       <c r="E2" s="2">
-        <f>C2-B2</f>
-        <v>2.0833333333333315E-2</v>
+        <f t="shared" ref="E2:E7" si="0">C2-B2</f>
+        <v>2.0833333333333426E-2</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -2999,12 +2996,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>44901</v>
       </c>
       <c r="B3" s="5">
-        <v>0.7753472222222223</v>
+        <v>0.77534722222222219</v>
       </c>
       <c r="C3" s="5">
         <v>0.827662037037037</v>
@@ -3013,8 +3010,8 @@
         <v>586</v>
       </c>
       <c r="E3" s="2">
-        <f>C3-B3</f>
-        <v>5.2314814814814703E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.2314814814814814E-2</v>
       </c>
       <c r="F3" s="6">
         <v>8</v>
@@ -3026,22 +3023,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>44902</v>
       </c>
       <c r="B4" s="5">
-        <v>0.12586805555555555</v>
+        <v>0.12586805555555561</v>
       </c>
       <c r="C4" s="5">
-        <v>0.19252314814814817</v>
+        <v>0.19252314814814811</v>
       </c>
       <c r="D4" s="7">
         <v>711</v>
       </c>
       <c r="E4" s="2">
-        <f>C4-B4</f>
-        <v>6.6655092592592613E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.6655092592592502E-2</v>
       </c>
       <c r="F4">
         <v>8</v>
@@ -3053,12 +3050,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>44903</v>
       </c>
       <c r="B5" s="5">
-        <v>0.74093749999999992</v>
+        <v>0.74093750000000003</v>
       </c>
       <c r="C5" s="5">
         <v>0.80609953703703707</v>
@@ -3067,8 +3064,8 @@
         <v>683</v>
       </c>
       <c r="E5" s="2">
-        <f>C5-B5</f>
-        <v>6.5162037037037157E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.5162037037037046E-2</v>
       </c>
       <c r="F5">
         <v>8</v>
@@ -3077,7 +3074,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>44914</v>
       </c>
@@ -3085,14 +3082,14 @@
         <v>0.59401620370370367</v>
       </c>
       <c r="C6" s="5">
-        <v>0.66849537037037043</v>
+        <v>0.66849537037037032</v>
       </c>
       <c r="D6">
         <v>455</v>
       </c>
       <c r="E6" s="2">
-        <f>C6-B6</f>
-        <v>7.4479166666666763E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.4479166666666652E-2</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -3101,7 +3098,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>44915</v>
       </c>
@@ -3115,7 +3112,7 @@
         <v>810</v>
       </c>
       <c r="E7" s="2">
-        <f>C7-B7</f>
+        <f t="shared" si="0"/>
         <v>7.9212962962962985E-2</v>
       </c>
       <c r="F7">
@@ -3127,12 +3124,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{3DC24ACB-B2DC-4D0E-A131-CE581BE59269}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{FB610B53-35CA-42A9-80B0-056C2FE2FF0F}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{EAC5AD3D-C5C2-49D2-BFA2-1BBC280BDF85}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{91ABD66D-FBD6-46B0-999A-04BA41F23D43}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{E7FE1CF4-C734-4A02-BFC3-650D65F7F1B9}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{D9A33521-75AF-4289-ACE3-18D37125EDE7}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3140,14 +3137,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D9C8E0-7D35-442F-8B31-E763EC1571B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A4" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -3158,7 +3155,7 @@
     <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -3184,15 +3181,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>44931</v>
       </c>
       <c r="B2" s="2">
-        <v>0.45209490740740743</v>
+        <v>0.45209490740740738</v>
       </c>
       <c r="C2" s="2">
-        <v>0.48959490740740735</v>
+        <v>0.48959490740740741</v>
       </c>
       <c r="D2">
         <v>302</v>
@@ -3212,7 +3209,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{75ED8EE8-3A4F-4C9D-AB6F-0CF2988A75E8}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: handle errors, logging, add classes
</commit_message>
<xml_diff>
--- a/Tiempos.xlsx
+++ b/Tiempos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Electrodomesticos" sheetId="1" state="visible" r:id="rId1"/>
@@ -3300,8 +3300,8 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3542,160 +3542,98 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A3:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col width="11.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="10.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="18" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="27.7109375" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="32.5703125" bestFit="1" customWidth="1" min="8" max="8"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Hora Inicio</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Hora Termino</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Cantidad</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Tiempo(HHMMSS)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Productos/min</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Enlace</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Observaciones</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>_hora_inicio</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>_fecha</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>_hora_fin</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>_cantidad</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>_tiempo</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>_productos_por_min</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>_enlace</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>_observaciones</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>_errores</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
-        <v>44931</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>0.4520949074074074</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>0.4895949074074074</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>14:15:06</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>08/01/2023</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>14:16:25</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>302</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0.0375</v>
+        <v>4</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0:01:19</t>
+        </is>
       </c>
       <c r="F2" t="n">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>fb_ropa_05-01-2023_302.xlsx</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Se extrae al día siguiente</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-01-05</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>21:34:48</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>21:36:07</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0:01:18</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>06/01/2023</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>23:39:27</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>23:40:32</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0:01:05</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Adición de mejoras
</commit_message>
<xml_diff>
--- a/Tiempos.xlsx
+++ b/Tiempos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BCRP\Codigos\GraphQL-Facebook-Marketplace-Ropa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6993890B-1FF7-4B16-A71C-E659B42FC2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66F9578-DCF9-4C3B-8652-C74FB61A9D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="64">
   <si>
     <t>Dia Semana</t>
   </si>
@@ -215,10 +215,19 @@
     <t>_enlace</t>
   </si>
   <si>
-    <t>_observaciones</t>
-  </si>
-  <si>
     <t>_errores</t>
+  </si>
+  <si>
+    <t>09:29:14</t>
+  </si>
+  <si>
+    <t>09/01/2023</t>
+  </si>
+  <si>
+    <t>11:06:48</t>
+  </si>
+  <si>
+    <t>1:37:33</t>
   </si>
 </sst>
 </file>
@@ -3159,15 +3168,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -3192,8 +3201,28 @@
       <c r="H1" t="s">
         <v>59</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <v>384</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejorando logica del codigo y agregando comentarios
</commit_message>
<xml_diff>
--- a/Tiempos.xlsx
+++ b/Tiempos.xlsx
@@ -3550,7 +3550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -4328,6 +4328,43 @@
         <v>1</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>02/02/2023</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>01:14:41</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>01:56:25</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>284</v>
+      </c>
+      <c r="E21" t="n">
+        <v>327</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0:41:43</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>6.81</v>
+      </c>
+      <c r="H21" t="n">
+        <v>7.84</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>